<commit_message>
Edits to Global and PS tests
</commit_message>
<xml_diff>
--- a/Product Sales/Product Setup/Main.rvl.xlsx
+++ b/Product Sales/Product Setup/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t>Flow</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>C:\UX365RegressionTest\Product Sales\Create sales non-inventory product\Main.rvl.xlsx</t>
+  </si>
+  <si>
+    <t>C:\UX365RegressionTest\Global\Open test Org\Main.rvl.xlsx</t>
+  </si>
+  <si>
+    <t>********Run Test: Open test Org*******</t>
   </si>
 </sst>
 </file>
@@ -609,7 +615,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -630,7 +636,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H4" s="40"/>
     </row>

</xml_diff>